<commit_message>
Add introspected annotation to ErrorTelegram.
</commit_message>
<xml_diff>
--- a/blanco-meta/telegrams/ErrorTelegram.xlsx
+++ b/blanco-meta/telegrams/ErrorTelegram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-api-core/blanco-meta/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9E2836-6088-5C44-B627-3367684A5862}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD90DCC-0FB6-BE41-852A-D58DC9463B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="3100" windowWidth="24240" windowHeight="13740" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
   <si>
     <t>クラス名</t>
   </si>
@@ -467,6 +467,10 @@
   </si>
   <si>
     <t>io.micronaut.core.annotation.Introspected</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>@Introspected</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1421,7 +1425,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1647,6 +1651,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2061,7 +2066,7 @@
   <dimension ref="A1:U51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:B30"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2185,7 +2190,9 @@
         <v>54</v>
       </c>
       <c r="B11" s="80"/>
-      <c r="C11" s="8"/>
+      <c r="C11" s="107" t="s">
+        <v>76</v>
+      </c>
       <c r="D11" s="35"/>
       <c r="E11" s="81"/>
       <c r="F11" s="75"/>

</xml_diff>

<commit_message>
* Dependencies for jackson related modules are defined as "api" for transit or prpagate depencendies to each project. * Add micronaut-serde-jackson for serialize/deserialize telegrams.
</commit_message>
<xml_diff>
--- a/blanco-meta/telegrams/ErrorTelegram.xlsx
+++ b/blanco-meta/telegrams/ErrorTelegram.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-api-core/blanco-meta/telegrams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD90DCC-0FB6-BE41-852A-D58DC9463B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7028803C-C008-8244-AFA9-915290F49101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4560" yWindow="3100" windowWidth="24240" windowHeight="13740" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="78">
   <si>
     <t>クラス名</t>
   </si>
@@ -470,7 +470,12 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>@Introspected</t>
+    <t>@Introspected
+@Serdeable</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>io.micronaut.serde.annotation.Serdeable</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1651,7 +1656,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="65" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -2063,10 +2070,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U51"/>
+  <dimension ref="A1:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2185,7 +2192,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" ht="30">
       <c r="A11" s="51" t="s">
         <v>54</v>
       </c>
@@ -2520,8 +2527,12 @@
       <c r="O30"/>
     </row>
     <row r="31" spans="1:18">
-      <c r="A31" s="57"/>
-      <c r="B31" s="58"/>
+      <c r="A31" s="57">
+        <v>2</v>
+      </c>
+      <c r="B31" s="58" t="s">
+        <v>77</v>
+      </c>
       <c r="C31" s="60"/>
       <c r="D31" s="60"/>
       <c r="E31" s="60"/>
@@ -2535,240 +2546,232 @@
       <c r="O31"/>
     </row>
     <row r="32" spans="1:18">
-      <c r="A32" s="61"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="79"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="78"/>
       <c r="G32" s="73"/>
       <c r="H32" s="73"/>
       <c r="I32" s="73"/>
       <c r="J32" s="73"/>
-      <c r="K32" s="71"/>
       <c r="M32"/>
       <c r="N32"/>
       <c r="O32"/>
     </row>
     <row r="33" spans="1:21">
-      <c r="A33"/>
-      <c r="B33"/>
-      <c r="C33"/>
-      <c r="D33"/>
-      <c r="E33"/>
-      <c r="F33"/>
-      <c r="G33"/>
-      <c r="H33"/>
-      <c r="I33"/>
-      <c r="J33"/>
-      <c r="K33" s="73"/>
-      <c r="L33"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="63"/>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="79"/>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73"/>
+      <c r="I33" s="73"/>
+      <c r="J33" s="73"/>
+      <c r="K33" s="71"/>
       <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
     </row>
     <row r="34" spans="1:21">
-      <c r="A34" s="3" t="s">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34" s="73"/>
+      <c r="L34"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="1:21">
+      <c r="A35" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
-      <c r="K34" s="67"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
-      <c r="N34" s="10"/>
-      <c r="O34" s="10"/>
-      <c r="P34" s="10"/>
-      <c r="Q34" s="10"/>
-      <c r="R34" s="10"/>
-      <c r="S34" s="10"/>
-      <c r="T34" s="5"/>
-      <c r="U34" s="11"/>
-    </row>
-    <row r="35" spans="1:21" ht="13.5" customHeight="1">
-      <c r="A35" s="94" t="s">
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="67"/>
+      <c r="H35" s="67"/>
+      <c r="I35" s="67"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="67"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="11"/>
+    </row>
+    <row r="36" spans="1:21" ht="13.5" customHeight="1">
+      <c r="A36" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="94" t="s">
+      <c r="B36" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="93" t="s">
+      <c r="C36" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="93" t="s">
+      <c r="D36" s="93" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="97" t="s">
+      <c r="E36" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="F35" s="95" t="s">
+      <c r="F36" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="104" t="s">
+      <c r="G36" s="104" t="s">
         <v>64</v>
       </c>
-      <c r="H35" s="104" t="s">
+      <c r="H36" s="104" t="s">
         <v>65</v>
       </c>
-      <c r="I35" s="102" t="s">
+      <c r="I36" s="102" t="s">
         <v>55</v>
       </c>
-      <c r="J35" s="101" t="s">
+      <c r="J36" s="101" t="s">
         <v>51</v>
       </c>
-      <c r="K35" s="105" t="s">
+      <c r="K36" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="L35" s="99" t="s">
+      <c r="L36" s="99" t="s">
         <v>20</v>
       </c>
-      <c r="M35" s="100"/>
-      <c r="N35" s="99" t="s">
+      <c r="M36" s="100"/>
+      <c r="N36" s="99" t="s">
         <v>21</v>
       </c>
-      <c r="O35" s="100"/>
-      <c r="P35" s="36" t="s">
+      <c r="O36" s="100"/>
+      <c r="P36" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="Q35" s="93" t="s">
+      <c r="Q36" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="R35" s="93"/>
-      <c r="S35" s="12"/>
-      <c r="T35" s="13"/>
-      <c r="U35" s="7"/>
-    </row>
-    <row r="36" spans="1:21">
-      <c r="A36" s="94"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="98"/>
-      <c r="F36" s="96"/>
-      <c r="G36" s="104"/>
-      <c r="H36" s="104"/>
-      <c r="I36" s="103"/>
-      <c r="J36" s="101"/>
-      <c r="K36" s="106"/>
-      <c r="L36" s="37" t="s">
+      <c r="R36" s="93"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="13"/>
+      <c r="U36" s="7"/>
+    </row>
+    <row r="37" spans="1:21">
+      <c r="A37" s="94"/>
+      <c r="B37" s="94"/>
+      <c r="C37" s="93"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="98"/>
+      <c r="F37" s="96"/>
+      <c r="G37" s="104"/>
+      <c r="H37" s="104"/>
+      <c r="I37" s="103"/>
+      <c r="J37" s="101"/>
+      <c r="K37" s="106"/>
+      <c r="L37" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="M36" s="37" t="s">
+      <c r="M37" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="N36" s="37" t="s">
+      <c r="N37" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="O36" s="37" t="s">
+      <c r="O37" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="P36" s="37" t="s">
+      <c r="P37" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="Q36" s="93"/>
-      <c r="R36" s="93"/>
-      <c r="S36" s="14"/>
-      <c r="T36" s="26"/>
-      <c r="U36" s="11"/>
-    </row>
-    <row r="37" spans="1:21">
-      <c r="A37" s="15">
-        <v>1</v>
-      </c>
-      <c r="B37" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70" t="s">
-        <v>56</v>
-      </c>
-      <c r="J37" s="68" t="s">
-        <v>41</v>
-      </c>
-      <c r="K37" s="87" t="s">
-        <v>41</v>
-      </c>
-      <c r="L37" s="38"/>
-      <c r="M37" s="39"/>
-      <c r="N37" s="38"/>
-      <c r="O37" s="39"/>
-      <c r="P37" s="40"/>
-      <c r="Q37" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="25"/>
+      <c r="Q37" s="93"/>
+      <c r="R37" s="93"/>
+      <c r="S37" s="14"/>
+      <c r="T37" s="26"/>
       <c r="U37" s="11"/>
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="15">
-        <f>A37+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>69</v>
+        <v>14</v>
       </c>
       <c r="C38" s="17" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="J38" s="69" t="s">
+      <c r="F38" s="70"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="70"/>
+      <c r="I38" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="J38" s="68" t="s">
         <v>41</v>
       </c>
       <c r="K38" s="87" t="s">
         <v>41</v>
       </c>
-      <c r="L38" s="27"/>
-      <c r="M38" s="27"/>
-      <c r="N38" s="27"/>
-      <c r="O38" s="27"/>
-      <c r="P38" s="27"/>
+      <c r="L38" s="38"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="38"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="40"/>
       <c r="Q38" s="17" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="R38" s="18"/>
       <c r="S38" s="18"/>
-      <c r="T38" s="19"/>
+      <c r="T38" s="25"/>
       <c r="U38" s="11"/>
     </row>
     <row r="39" spans="1:21">
-      <c r="A39" s="15"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
+      <c r="A39" s="15">
+        <f>A38+1</f>
+        <v>2</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>28</v>
+      </c>
       <c r="D39" s="17"/>
       <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
+      <c r="F39" s="27"/>
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-      <c r="J39" s="69"/>
-      <c r="K39" s="87"/>
-      <c r="L39" s="17"/>
-      <c r="M39" s="17"/>
-      <c r="N39" s="17"/>
-      <c r="O39" s="17"/>
-      <c r="P39" s="17"/>
-      <c r="Q39" s="17"/>
+      <c r="I39" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="J39" s="69" t="s">
+        <v>41</v>
+      </c>
+      <c r="K39" s="87" t="s">
+        <v>41</v>
+      </c>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="R39" s="18"/>
       <c r="S39" s="18"/>
       <c r="T39" s="19"/>
@@ -2803,17 +2806,17 @@
       <c r="C41" s="17"/>
       <c r="D41" s="17"/>
       <c r="E41" s="17"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
+      <c r="F41" s="17"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+      <c r="J41" s="69"/>
       <c r="K41" s="87"/>
-      <c r="L41" s="27"/>
-      <c r="M41" s="27"/>
-      <c r="N41" s="27"/>
-      <c r="O41" s="27"/>
-      <c r="P41" s="27"/>
+      <c r="L41" s="17"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
       <c r="Q41" s="17"/>
       <c r="R41" s="18"/>
       <c r="S41" s="18"/>
@@ -2826,17 +2829,17 @@
       <c r="C42" s="17"/>
       <c r="D42" s="17"/>
       <c r="E42" s="17"/>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-      <c r="J42" s="17"/>
+      <c r="F42" s="27"/>
+      <c r="G42" s="27"/>
+      <c r="H42" s="27"/>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
       <c r="K42" s="87"/>
-      <c r="L42" s="17"/>
-      <c r="M42" s="17"/>
-      <c r="N42" s="17"/>
-      <c r="O42" s="17"/>
-      <c r="P42" s="17"/>
+      <c r="L42" s="27"/>
+      <c r="M42" s="27"/>
+      <c r="N42" s="27"/>
+      <c r="O42" s="27"/>
+      <c r="P42" s="27"/>
       <c r="Q42" s="17"/>
       <c r="R42" s="18"/>
       <c r="S42" s="18"/>
@@ -2850,10 +2853,10 @@
       <c r="D43" s="17"/>
       <c r="E43" s="17"/>
       <c r="F43" s="17"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
       <c r="K43" s="87"/>
       <c r="L43" s="17"/>
       <c r="M43" s="17"/>
@@ -2873,10 +2876,10 @@
       <c r="D44" s="17"/>
       <c r="E44" s="17"/>
       <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
-      <c r="J44" s="17"/>
+      <c r="G44" s="27"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
       <c r="K44" s="87"/>
       <c r="L44" s="17"/>
       <c r="M44" s="17"/>
@@ -2896,10 +2899,10 @@
       <c r="D45" s="17"/>
       <c r="E45" s="17"/>
       <c r="F45" s="17"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+      <c r="J45" s="17"/>
       <c r="K45" s="87"/>
       <c r="L45" s="17"/>
       <c r="M45" s="17"/>
@@ -2919,10 +2922,10 @@
       <c r="D46" s="17"/>
       <c r="E46" s="17"/>
       <c r="F46" s="17"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
-      <c r="J46" s="17"/>
+      <c r="G46" s="27"/>
+      <c r="H46" s="27"/>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
       <c r="K46" s="87"/>
       <c r="L46" s="17"/>
       <c r="M46" s="17"/>
@@ -2936,30 +2939,50 @@
       <c r="U46" s="11"/>
     </row>
     <row r="47" spans="1:21">
-      <c r="A47" s="20"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="22"/>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
-      <c r="F47" s="22"/>
-      <c r="G47" s="88"/>
-      <c r="H47" s="88"/>
-      <c r="I47" s="82"/>
-      <c r="J47" s="82"/>
-      <c r="K47" s="89"/>
-      <c r="L47" s="22"/>
-      <c r="M47" s="22"/>
-      <c r="N47" s="22"/>
-      <c r="O47" s="22"/>
-      <c r="P47" s="22"/>
-      <c r="Q47" s="22"/>
-      <c r="R47" s="23"/>
-      <c r="S47" s="23"/>
-      <c r="T47" s="24"/>
+      <c r="A47" s="15"/>
+      <c r="B47" s="16"/>
+      <c r="C47" s="17"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+      <c r="K47" s="87"/>
+      <c r="L47" s="17"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="19"/>
       <c r="U47" s="11"/>
     </row>
     <row r="48" spans="1:21">
-      <c r="K48" s="90"/>
+      <c r="A48" s="20"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="22"/>
+      <c r="D48" s="22"/>
+      <c r="E48" s="22"/>
+      <c r="F48" s="22"/>
+      <c r="G48" s="88"/>
+      <c r="H48" s="88"/>
+      <c r="I48" s="82"/>
+      <c r="J48" s="82"/>
+      <c r="K48" s="89"/>
+      <c r="L48" s="22"/>
+      <c r="M48" s="22"/>
+      <c r="N48" s="22"/>
+      <c r="O48" s="22"/>
+      <c r="P48" s="22"/>
+      <c r="Q48" s="22"/>
+      <c r="R48" s="23"/>
+      <c r="S48" s="23"/>
+      <c r="T48" s="24"/>
+      <c r="U48" s="11"/>
     </row>
     <row r="49" spans="11:11">
       <c r="K49" s="90"/>
@@ -2969,28 +2992,31 @@
     </row>
     <row r="51" spans="11:11">
       <c r="K51" s="90"/>
+    </row>
+    <row r="52" spans="11:11">
+      <c r="K52" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="Q35:R36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="L35:M35"/>
-    <mergeCell ref="N35:O35"/>
-    <mergeCell ref="J35:J36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="K35:K36"/>
+    <mergeCell ref="Q36:R37"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="C36:C37"/>
+    <mergeCell ref="F36:F37"/>
+    <mergeCell ref="D36:D37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="L36:M36"/>
+    <mergeCell ref="N36:O36"/>
+    <mergeCell ref="J36:J37"/>
+    <mergeCell ref="I36:I37"/>
+    <mergeCell ref="G36:G37"/>
+    <mergeCell ref="H36:H37"/>
+    <mergeCell ref="K36:K37"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
-  <dataValidations count="9">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L49:P49 F59 K62" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations disablePrompts="1" count="9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="L50:P50 F60 K63" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3003,7 +3029,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C20" xr:uid="{F37E9BBA-0828-7A47-894D-CEEBF6D9B23D}">
       <formula1>adjustDefaultValue</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J37:J47" xr:uid="{AF2A87C6-B9B6-7F46-A27A-581DA97035E2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J38:J48" xr:uid="{AF2A87C6-B9B6-7F46-A27A-581DA97035E2}">
       <formula1>others</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14" xr:uid="{40B4C319-B08C-464C-B234-307EFE76C1B7}">

</xml_diff>